<commit_message>
API-430 add interface comments, add log to file
</commit_message>
<xml_diff>
--- a/TestRTD0.xlsx
+++ b/TestRTD0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\hello_rtd_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0091C82-F7B3-4969-91CE-089E647D836C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCA03A7-AB73-489E-886E-05BEA5A1A5D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6660" yWindow="210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
   <volType type="realTimeData">
     <main first="hello_rtd_excel">
       <tp t="s">
-        <v>data from hello_rtd_excel_0: 76</v>
+        <v>data from hello_rtd_excel_0: 88</v>
         <stp/>
         <stp>AAA</stp>
         <stp>1</stp>
@@ -372,7 +372,7 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>RTD("hello_rtd_excel", , "AAA", 1)</f>
-        <v>data from hello_rtd_excel_0: 76</v>
+        <v>data from hello_rtd_excel_0: 88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API-430 add json package
</commit_message>
<xml_diff>
--- a/TestRTD0.xlsx
+++ b/TestRTD0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\hello_rtd_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCA03A7-AB73-489E-886E-05BEA5A1A5D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800EC688-342E-4466-83AF-32AF282CAB4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6660" yWindow="210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
   <volType type="realTimeData">
     <main first="hello_rtd_excel">
       <tp t="s">
-        <v>data from hello_rtd_excel_0: 88</v>
+        <v>data from hello_rtd_excel_0: 33</v>
         <stp/>
         <stp>AAA</stp>
         <stp>1</stp>
@@ -363,16 +363,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>RTD("hello_rtd_excel", , "AAA", 1)</f>
-        <v>data from hello_rtd_excel_0: 88</v>
+        <v>data from hello_rtd_excel_0: 33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API-430 return data by topic
</commit_message>
<xml_diff>
--- a/TestRTD0.xlsx
+++ b/TestRTD0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\hello_rtd_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800EC688-342E-4466-83AF-32AF282CAB4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE3B3EC-DF22-4C90-AAA8-7D6FBD62657A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6660" yWindow="210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,6 +30,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>ACB</t>
+  </si>
+  <si>
+    <t>VCS</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -87,11 +98,18 @@
   <volType type="realTimeData">
     <main first="hello_rtd_excel">
       <tp t="s">
-        <v>data from hello_rtd_excel_0: 33</v>
+        <v>data from hello_rtd_excel for topic ACB at 2020-05-19T06:29:38.2204955Z:  2</v>
         <stp/>
-        <stp>AAA</stp>
+        <stp>ACB</stp>
         <stp>1</stp>
-        <tr r="A1" s="1"/>
+        <tr r="B1" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>data from hello_rtd_excel for topic VCS at 2020-05-19T06:29:38.2204955Z:  75</v>
+        <stp/>
+        <stp>VCS</stp>
+        <stp>1</stp>
+        <tr r="B2" s="1"/>
       </tp>
     </main>
   </volType>
@@ -361,16 +379,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O27" sqref="N27:O27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
-        <f>RTD("hello_rtd_excel", , "AAA", 1)</f>
-        <v>data from hello_rtd_excel_0: 33</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="str">
+        <f>RTD("hello_rtd_excel", , "ACB",1)</f>
+        <v>data from hello_rtd_excel for topic ACB at 2020-05-19T06:29:38.2204955Z:  2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>RTD("hello_rtd_excel", , "VCS",1)</f>
+        <v>data from hello_rtd_excel for topic VCS at 2020-05-19T06:29:38.2204955Z:  75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API-430 improve data update
</commit_message>
<xml_diff>
--- a/TestRTD0.xlsx
+++ b/TestRTD0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\hello_rtd_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E967D552-A866-47F4-9626-5045655FA010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7171E81F-981F-4ECB-9640-1D0CE07C0C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,15 +97,15 @@
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
     <main first="hello_rtd_excel">
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>ACB's data is not available</v>
         <stp/>
         <stp>ACB</stp>
         <stp>1</stp>
         <tr r="B1" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>VCS's data is not available</v>
         <stp/>
         <stp>VCS</stp>
         <stp>1</stp>
@@ -393,16 +393,16 @@
       </c>
       <c r="B1" t="str">
         <f>RTD("hello_rtd_excel", , "ACB",1)</f>
-        <v>data from hello_rtd_excel for topic ACB at 2020-05-19T07:32:25.5013387Z:  63</v>
+        <v>ACB's data is not available</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="e">
+      <c r="B2" t="str">
         <f>RTD("hello_rtd_excel", , "VCS",1)</f>
-        <v>#N/A</v>
+        <v>VCS's data is not available</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API-430 improve data update 2
</commit_message>
<xml_diff>
--- a/TestRTD0.xlsx
+++ b/TestRTD0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\hello_rtd_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7171E81F-981F-4ECB-9640-1D0CE07C0C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D0A41A-AB69-478A-A950-FD3CB6CA03B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3870" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,14 +98,14 @@
   <volType type="realTimeData">
     <main first="hello_rtd_excel">
       <tp t="s">
-        <v>ACB's data is not available</v>
+        <v>{"code":null,"referencePrice":22000.0,"last":20900.0,"change":-1100.0,"bidPrice":0.0,"bidVolume":0.0}</v>
         <stp/>
         <stp>ACB</stp>
         <stp>1</stp>
         <tr r="B1" s="1"/>
       </tp>
       <tp t="s">
-        <v>VCS's data is not available</v>
+        <v>{"code":null,"referencePrice":0.0,"last":0.0,"change":0.0,"bidPrice":0.0,"bidVolume":0.0}</v>
         <stp/>
         <stp>VCS</stp>
         <stp>1</stp>
@@ -393,7 +393,7 @@
       </c>
       <c r="B1" t="str">
         <f>RTD("hello_rtd_excel", , "ACB",1)</f>
-        <v>ACB's data is not available</v>
+        <v>{"code":null,"referencePrice":22000.0,"last":20900.0,"change":-1100.0,"bidPrice":0.0,"bidVolume":0.0}</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -402,7 +402,7 @@
       </c>
       <c r="B2" t="str">
         <f>RTD("hello_rtd_excel", , "VCS",1)</f>
-        <v>VCS's data is not available</v>
+        <v>{"code":null,"referencePrice":0.0,"last":0.0,"change":0.0,"bidPrice":0.0,"bidVolume":0.0}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>